<commit_message>
Update CU Config data file
</commit_message>
<xml_diff>
--- a/apps/management/data/cuconfig.xlsx
+++ b/apps/management/data/cuconfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\KULIAH\CAPSTONE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8EB8AC-DB3B-4C33-B231-8104332C80DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981C0EE1-D561-4166-A529-B426AD1ABF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B64A2D01-6A8A-4003-9F69-1613FCC59EE7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="142">
   <si>
     <t>12345678L</t>
   </si>
@@ -401,9 +401,6 @@
     <t>172.21.8.118</t>
   </si>
   <si>
-    <t>172.21.6.122</t>
-  </si>
-  <si>
     <t>0xe30</t>
   </si>
   <si>
@@ -413,9 +410,6 @@
     <t>172.21.8.119</t>
   </si>
   <si>
-    <t>172.21.6.123</t>
-  </si>
-  <si>
     <t>0xe31</t>
   </si>
   <si>
@@ -425,9 +419,6 @@
     <t>172.21.8.120</t>
   </si>
   <si>
-    <t>172.21.6.124</t>
-  </si>
-  <si>
     <t>0xe32</t>
   </si>
   <si>
@@ -435,9 +426,6 @@
   </si>
   <si>
     <t>172.21.8.121</t>
-  </si>
-  <si>
-    <t>172.21.6.125</t>
   </si>
   <si>
     <t>cuid</t>
@@ -480,7 +468,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,6 +480,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -885,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78109DB-9D3D-4624-8643-4B2CAB067356}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,40 +890,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1005,7 +999,7 @@
         <v>1</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1043,7 +1037,7 @@
         <v>1</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1081,7 +1075,7 @@
         <v>1</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1119,7 +1113,7 @@
         <v>1</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1157,7 +1151,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1195,7 +1189,7 @@
         <v>1</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1233,7 +1227,7 @@
         <v>1</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1271,7 +1265,7 @@
         <v>1</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1309,7 +1303,7 @@
         <v>1</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1347,7 +1341,7 @@
         <v>1</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1385,7 +1379,7 @@
         <v>1</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1423,7 +1417,7 @@
         <v>1</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1461,7 +1455,7 @@
         <v>1</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1499,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1537,7 +1531,7 @@
         <v>1</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>69</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1575,7 +1569,7 @@
         <v>1</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>73</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1613,7 +1607,7 @@
         <v>1</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1651,7 +1645,7 @@
         <v>1</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>81</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1689,7 +1683,7 @@
         <v>1</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>85</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1727,7 +1721,7 @@
         <v>1</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1765,7 +1759,7 @@
         <v>1</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1803,7 +1797,7 @@
         <v>1</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1841,7 +1835,7 @@
         <v>1</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1879,7 +1873,7 @@
         <v>1</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>105</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1917,7 +1911,7 @@
         <v>1</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>109</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1955,7 +1949,7 @@
         <v>1</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>113</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1993,7 +1987,7 @@
         <v>1</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>117</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2031,18 +2025,18 @@
         <v>1</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>121</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="D31" s="2">
         <v>2152</v>
@@ -2054,7 +2048,7 @@
         <v>109</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H31" s="3">
         <v>208</v>
@@ -2069,18 +2063,18 @@
         <v>1</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>125</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D32" s="2">
         <v>2152</v>
@@ -2092,7 +2086,7 @@
         <v>113</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H32" s="3">
         <v>208</v>
@@ -2107,18 +2101,18 @@
         <v>1</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D33" s="2">
         <v>2152</v>
@@ -2130,7 +2124,7 @@
         <v>117</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H33" s="3">
         <v>208</v>
@@ -2145,10 +2139,11 @@
         <v>1</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>133</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update on cuconfig file
</commit_message>
<xml_diff>
--- a/apps/management/data/cuconfig.xlsx
+++ b/apps/management/data/cuconfig.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\KULIAH\CAPSTONE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981C0EE1-D561-4166-A529-B426AD1ABF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8632FE1C-9F60-4D66-BC57-6F6B164929EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B64A2D01-6A8A-4003-9F69-1613FCC59EE7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="143">
   <si>
     <t>12345678L</t>
   </si>
@@ -50,12 +50,6 @@
     <t>0xe01</t>
   </si>
   <si>
-    <t>172.21.6.90</t>
-  </si>
-  <si>
-    <t>172.21.8.90</t>
-  </si>
-  <si>
     <t>172.21.6.94</t>
   </si>
   <si>
@@ -65,369 +59,186 @@
     <t>192.168.1.9</t>
   </si>
   <si>
-    <t>172.21.6.91</t>
-  </si>
-  <si>
-    <t>172.21.8.91</t>
-  </si>
-  <si>
-    <t>172.21.6.95</t>
-  </si>
-  <si>
     <t>0xe03</t>
   </si>
   <si>
     <t>192.168.1.17</t>
   </si>
   <si>
-    <t>172.21.6.92</t>
-  </si>
-  <si>
-    <t>172.21.8.92</t>
-  </si>
-  <si>
-    <t>172.21.6.96</t>
-  </si>
-  <si>
     <t>0xe04</t>
   </si>
   <si>
     <t>192.168.1.25</t>
   </si>
   <si>
-    <t>172.21.6.93</t>
-  </si>
-  <si>
-    <t>172.21.8.93</t>
-  </si>
-  <si>
-    <t>172.21.6.97</t>
-  </si>
-  <si>
     <t>0xe05</t>
   </si>
   <si>
     <t>192.168.1.33</t>
   </si>
   <si>
-    <t>172.21.8.94</t>
-  </si>
-  <si>
-    <t>172.21.6.98</t>
-  </si>
-  <si>
     <t>0xe06</t>
   </si>
   <si>
     <t>192.168.1.41</t>
   </si>
   <si>
-    <t>172.21.8.95</t>
-  </si>
-  <si>
-    <t>172.21.6.99</t>
-  </si>
-  <si>
     <t>0xe07</t>
   </si>
   <si>
     <t>192.168.1.49</t>
   </si>
   <si>
-    <t>172.21.8.96</t>
-  </si>
-  <si>
-    <t>172.21.6.100</t>
-  </si>
-  <si>
     <t>0xe08</t>
   </si>
   <si>
     <t>192.168.1.57</t>
   </si>
   <si>
-    <t>172.21.8.97</t>
-  </si>
-  <si>
-    <t>172.21.6.101</t>
-  </si>
-  <si>
     <t>0xe09</t>
   </si>
   <si>
     <t>192.168.1.65</t>
   </si>
   <si>
-    <t>172.21.8.98</t>
-  </si>
-  <si>
-    <t>172.21.6.102</t>
-  </si>
-  <si>
     <t>0xe10</t>
   </si>
   <si>
     <t>192.168.1.73</t>
   </si>
   <si>
-    <t>172.21.8.99</t>
-  </si>
-  <si>
-    <t>172.21.6.103</t>
-  </si>
-  <si>
     <t>0xe11</t>
   </si>
   <si>
     <t>192.168.1.81</t>
   </si>
   <si>
-    <t>172.21.8.100</t>
-  </si>
-  <si>
-    <t>172.21.6.104</t>
-  </si>
-  <si>
     <t>0xe12</t>
   </si>
   <si>
     <t>192.168.1.89</t>
   </si>
   <si>
-    <t>172.21.8.101</t>
-  </si>
-  <si>
-    <t>172.21.6.105</t>
-  </si>
-  <si>
     <t>0xe13</t>
   </si>
   <si>
     <t>192.168.1.97</t>
   </si>
   <si>
-    <t>172.21.8.102</t>
-  </si>
-  <si>
-    <t>172.21.6.106</t>
-  </si>
-  <si>
     <t>0xe14</t>
   </si>
   <si>
     <t>192.168.1.105</t>
   </si>
   <si>
-    <t>172.21.8.103</t>
-  </si>
-  <si>
-    <t>172.21.6.107</t>
-  </si>
-  <si>
     <t>0xe15</t>
   </si>
   <si>
     <t>192.168.1.113</t>
   </si>
   <si>
-    <t>172.21.8.104</t>
-  </si>
-  <si>
-    <t>172.21.6.108</t>
-  </si>
-  <si>
     <t>0xe16</t>
   </si>
   <si>
     <t>192.168.1.121</t>
   </si>
   <si>
-    <t>172.21.8.105</t>
-  </si>
-  <si>
-    <t>172.21.6.109</t>
-  </si>
-  <si>
     <t>0xe17</t>
   </si>
   <si>
     <t>192.168.1.129</t>
   </si>
   <si>
-    <t>172.21.8.106</t>
-  </si>
-  <si>
-    <t>172.21.6.110</t>
-  </si>
-  <si>
     <t>0xe18</t>
   </si>
   <si>
     <t>192.168.1.137</t>
   </si>
   <si>
-    <t>172.21.8.107</t>
-  </si>
-  <si>
-    <t>172.21.6.111</t>
-  </si>
-  <si>
     <t>0xe19</t>
   </si>
   <si>
     <t>192.168.1.145</t>
   </si>
   <si>
-    <t>172.21.8.108</t>
-  </si>
-  <si>
-    <t>172.21.6.112</t>
-  </si>
-  <si>
     <t>0xe20</t>
   </si>
   <si>
     <t>192.168.1.153</t>
   </si>
   <si>
-    <t>172.21.8.109</t>
-  </si>
-  <si>
-    <t>172.21.6.113</t>
-  </si>
-  <si>
     <t>0xe21</t>
   </si>
   <si>
     <t>192.168.1.161</t>
   </si>
   <si>
-    <t>172.21.8.110</t>
-  </si>
-  <si>
-    <t>172.21.6.114</t>
-  </si>
-  <si>
     <t>0xe22</t>
   </si>
   <si>
     <t>192.168.1.169</t>
   </si>
   <si>
-    <t>172.21.8.111</t>
-  </si>
-  <si>
-    <t>172.21.6.115</t>
-  </si>
-  <si>
     <t>0xe23</t>
   </si>
   <si>
     <t>192.168.1.177</t>
   </si>
   <si>
-    <t>172.21.8.112</t>
-  </si>
-  <si>
-    <t>172.21.6.116</t>
-  </si>
-  <si>
     <t>0xe24</t>
   </si>
   <si>
     <t>192.168.1.185</t>
   </si>
   <si>
-    <t>172.21.8.113</t>
-  </si>
-  <si>
-    <t>172.21.6.117</t>
-  </si>
-  <si>
     <t>0xe25</t>
   </si>
   <si>
     <t>192.168.1.193</t>
   </si>
   <si>
-    <t>172.21.8.114</t>
-  </si>
-  <si>
-    <t>172.21.6.118</t>
-  </si>
-  <si>
     <t>0xe26</t>
   </si>
   <si>
     <t>192.168.1.201</t>
   </si>
   <si>
-    <t>172.21.8.115</t>
-  </si>
-  <si>
-    <t>172.21.6.119</t>
-  </si>
-  <si>
     <t>0xe27</t>
   </si>
   <si>
     <t>192.168.1.209</t>
   </si>
   <si>
-    <t>172.21.8.116</t>
-  </si>
-  <si>
-    <t>172.21.6.120</t>
-  </si>
-  <si>
     <t>0xe28</t>
   </si>
   <si>
     <t>192.168.1.217</t>
   </si>
   <si>
-    <t>172.21.8.117</t>
-  </si>
-  <si>
-    <t>172.21.6.121</t>
-  </si>
-  <si>
     <t>0xe29</t>
   </si>
   <si>
     <t>192.168.1.225</t>
   </si>
   <si>
-    <t>172.21.8.118</t>
-  </si>
-  <si>
     <t>0xe30</t>
   </si>
   <si>
     <t>192.168.1.233</t>
   </si>
   <si>
-    <t>172.21.8.119</t>
-  </si>
-  <si>
     <t>0xe31</t>
   </si>
   <si>
     <t>192.168.1.241</t>
   </si>
   <si>
-    <t>172.21.8.120</t>
-  </si>
-  <si>
     <t>0xe32</t>
   </si>
   <si>
     <t>192.168.1.249</t>
   </si>
   <si>
-    <t>172.21.8.121</t>
-  </si>
-  <si>
     <t>cuid</t>
   </si>
   <si>
@@ -462,13 +273,205 @@
   </si>
   <si>
     <t>f1duport</t>
+  </si>
+  <si>
+    <t>172.21.6.1</t>
+  </si>
+  <si>
+    <t>172.21.6.2</t>
+  </si>
+  <si>
+    <t>172.21.6.3</t>
+  </si>
+  <si>
+    <t>172.21.6.4</t>
+  </si>
+  <si>
+    <t>172.21.6.5</t>
+  </si>
+  <si>
+    <t>172.21.6.6</t>
+  </si>
+  <si>
+    <t>172.21.6.7</t>
+  </si>
+  <si>
+    <t>172.21.6.8</t>
+  </si>
+  <si>
+    <t>172.21.6.9</t>
+  </si>
+  <si>
+    <t>172.21.6.10</t>
+  </si>
+  <si>
+    <t>172.21.6.11</t>
+  </si>
+  <si>
+    <t>172.21.6.12</t>
+  </si>
+  <si>
+    <t>172.21.6.13</t>
+  </si>
+  <si>
+    <t>172.21.6.14</t>
+  </si>
+  <si>
+    <t>172.21.6.15</t>
+  </si>
+  <si>
+    <t>172.21.6.16</t>
+  </si>
+  <si>
+    <t>172.21.6.17</t>
+  </si>
+  <si>
+    <t>172.21.6.18</t>
+  </si>
+  <si>
+    <t>172.21.6.19</t>
+  </si>
+  <si>
+    <t>172.21.6.20</t>
+  </si>
+  <si>
+    <t>172.21.6.21</t>
+  </si>
+  <si>
+    <t>172.21.6.22</t>
+  </si>
+  <si>
+    <t>172.21.6.23</t>
+  </si>
+  <si>
+    <t>172.21.6.24</t>
+  </si>
+  <si>
+    <t>172.21.6.25</t>
+  </si>
+  <si>
+    <t>172.21.6.26</t>
+  </si>
+  <si>
+    <t>172.21.6.27</t>
+  </si>
+  <si>
+    <t>172.21.6.28</t>
+  </si>
+  <si>
+    <t>172.21.6.29</t>
+  </si>
+  <si>
+    <t>172.21.6.30</t>
+  </si>
+  <si>
+    <t>172.21.6.31</t>
+  </si>
+  <si>
+    <t>172.21.6.32</t>
+  </si>
+  <si>
+    <t>172.21.8.1</t>
+  </si>
+  <si>
+    <t>172.21.8.2</t>
+  </si>
+  <si>
+    <t>172.21.8.3</t>
+  </si>
+  <si>
+    <t>172.21.8.4</t>
+  </si>
+  <si>
+    <t>172.21.8.5</t>
+  </si>
+  <si>
+    <t>172.21.8.6</t>
+  </si>
+  <si>
+    <t>172.21.8.7</t>
+  </si>
+  <si>
+    <t>172.21.8.8</t>
+  </si>
+  <si>
+    <t>172.21.8.9</t>
+  </si>
+  <si>
+    <t>172.21.8.10</t>
+  </si>
+  <si>
+    <t>172.21.8.11</t>
+  </si>
+  <si>
+    <t>172.21.8.12</t>
+  </si>
+  <si>
+    <t>172.21.8.13</t>
+  </si>
+  <si>
+    <t>172.21.8.14</t>
+  </si>
+  <si>
+    <t>172.21.8.15</t>
+  </si>
+  <si>
+    <t>172.21.8.16</t>
+  </si>
+  <si>
+    <t>172.21.8.17</t>
+  </si>
+  <si>
+    <t>172.21.8.18</t>
+  </si>
+  <si>
+    <t>172.21.8.19</t>
+  </si>
+  <si>
+    <t>172.21.8.20</t>
+  </si>
+  <si>
+    <t>172.21.8.21</t>
+  </si>
+  <si>
+    <t>172.21.8.22</t>
+  </si>
+  <si>
+    <t>172.21.8.23</t>
+  </si>
+  <si>
+    <t>172.21.8.24</t>
+  </si>
+  <si>
+    <t>172.21.8.25</t>
+  </si>
+  <si>
+    <t>172.21.8.26</t>
+  </si>
+  <si>
+    <t>172.21.8.27</t>
+  </si>
+  <si>
+    <t>172.21.8.28</t>
+  </si>
+  <si>
+    <t>172.21.8.29</t>
+  </si>
+  <si>
+    <t>172.21.8.30</t>
+  </si>
+  <si>
+    <t>172.21.8.31</t>
+  </si>
+  <si>
+    <t>172.21.8.32</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,6 +493,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -505,7 +514,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -528,11 +537,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -542,6 +590,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -879,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78109DB-9D3D-4624-8643-4B2CAB067356}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,40 +950,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>130</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>131</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>132</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>140</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>133</v>
+        <v>78</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>134</v>
+        <v>71</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>135</v>
+        <v>72</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>136</v>
+        <v>73</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>137</v>
+        <v>74</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>138</v>
+        <v>75</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>139</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -939,14 +999,14 @@
       <c r="D2" s="2">
         <v>2152</v>
       </c>
-      <c r="E2" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>5</v>
+      <c r="E2" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="H2" s="3">
         <v>208</v>
@@ -961,30 +1021,30 @@
         <v>1</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2">
         <v>2152</v>
       </c>
-      <c r="E3" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>10</v>
+      <c r="E3" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="H3" s="3">
         <v>208</v>
@@ -999,30 +1059,30 @@
         <v>1</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2">
         <v>2152</v>
       </c>
-      <c r="E4" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>15</v>
+      <c r="E4" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="H4" s="3">
         <v>208</v>
@@ -1037,30 +1097,30 @@
         <v>1</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2">
         <v>2152</v>
       </c>
-      <c r="E5" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>20</v>
+      <c r="E5" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="H5" s="3">
         <v>208</v>
@@ -1075,30 +1135,30 @@
         <v>1</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2">
         <v>2152</v>
       </c>
-      <c r="E6" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>24</v>
+      <c r="E6" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>115</v>
       </c>
       <c r="H6" s="3">
         <v>208</v>
@@ -1113,30 +1173,30 @@
         <v>1</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2">
         <v>2152</v>
       </c>
-      <c r="E7" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>28</v>
+      <c r="E7" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="H7" s="3">
         <v>208</v>
@@ -1151,30 +1211,30 @@
         <v>1</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2">
         <v>2152</v>
       </c>
-      <c r="E8" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>32</v>
+      <c r="E8" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="H8" s="3">
         <v>208</v>
@@ -1189,30 +1249,30 @@
         <v>1</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2">
         <v>2152</v>
       </c>
-      <c r="E9" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>36</v>
+      <c r="E9" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="H9" s="3">
         <v>208</v>
@@ -1227,30 +1287,30 @@
         <v>1</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2">
         <v>2152</v>
       </c>
-      <c r="E10" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>40</v>
+      <c r="E10" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="H10" s="3">
         <v>208</v>
@@ -1265,30 +1325,30 @@
         <v>1</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2">
         <v>2152</v>
       </c>
-      <c r="E11" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>44</v>
+      <c r="E11" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>120</v>
       </c>
       <c r="H11" s="3">
         <v>208</v>
@@ -1303,30 +1363,30 @@
         <v>1</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="D12" s="2">
         <v>2152</v>
       </c>
-      <c r="E12" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>48</v>
+      <c r="E12" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>121</v>
       </c>
       <c r="H12" s="3">
         <v>208</v>
@@ -1341,30 +1401,30 @@
         <v>1</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="D13" s="2">
         <v>2152</v>
       </c>
-      <c r="E13" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>52</v>
+      <c r="E13" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="H13" s="3">
         <v>208</v>
@@ -1379,30 +1439,30 @@
         <v>1</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="D14" s="2">
         <v>2152</v>
       </c>
-      <c r="E14" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>56</v>
+      <c r="E14" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="H14" s="3">
         <v>208</v>
@@ -1417,30 +1477,30 @@
         <v>1</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2">
         <v>2152</v>
       </c>
-      <c r="E15" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>60</v>
+      <c r="E15" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="H15" s="3">
         <v>208</v>
@@ -1455,30 +1515,30 @@
         <v>1</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="D16" s="2">
         <v>2152</v>
       </c>
-      <c r="E16" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>64</v>
+      <c r="E16" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="H16" s="3">
         <v>208</v>
@@ -1493,30 +1553,30 @@
         <v>1</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="D17" s="2">
         <v>2152</v>
       </c>
-      <c r="E17" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>68</v>
+      <c r="E17" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="H17" s="3">
         <v>208</v>
@@ -1531,30 +1591,30 @@
         <v>1</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="D18" s="2">
         <v>2152</v>
       </c>
-      <c r="E18" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>72</v>
+      <c r="E18" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>127</v>
       </c>
       <c r="H18" s="3">
         <v>208</v>
@@ -1569,30 +1629,30 @@
         <v>1</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2">
         <v>2152</v>
       </c>
-      <c r="E19" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>76</v>
+      <c r="E19" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>128</v>
       </c>
       <c r="H19" s="3">
         <v>208</v>
@@ -1607,30 +1667,30 @@
         <v>1</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="D20" s="2">
         <v>2152</v>
       </c>
-      <c r="E20" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>80</v>
+      <c r="E20" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="H20" s="3">
         <v>208</v>
@@ -1645,30 +1705,30 @@
         <v>1</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="D21" s="2">
         <v>2152</v>
       </c>
-      <c r="E21" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>84</v>
+      <c r="E21" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="H21" s="3">
         <v>208</v>
@@ -1683,30 +1743,30 @@
         <v>1</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="D22" s="2">
         <v>2152</v>
       </c>
-      <c r="E22" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>88</v>
+      <c r="E22" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H22" s="3">
         <v>208</v>
@@ -1721,30 +1781,30 @@
         <v>1</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="D23" s="2">
         <v>2152</v>
       </c>
-      <c r="E23" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>92</v>
+      <c r="E23" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="H23" s="3">
         <v>208</v>
@@ -1759,30 +1819,30 @@
         <v>1</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="D24" s="2">
         <v>2152</v>
       </c>
-      <c r="E24" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>96</v>
+      <c r="E24" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>133</v>
       </c>
       <c r="H24" s="3">
         <v>208</v>
@@ -1797,30 +1857,30 @@
         <v>1</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="D25" s="2">
         <v>2152</v>
       </c>
-      <c r="E25" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>100</v>
+      <c r="E25" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="H25" s="3">
         <v>208</v>
@@ -1835,30 +1895,30 @@
         <v>1</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="2">
+        <v>2152</v>
+      </c>
+      <c r="E26" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F26" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="2">
-        <v>2152</v>
-      </c>
-      <c r="E26" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>104</v>
+      <c r="G26" s="5" t="s">
+        <v>135</v>
       </c>
       <c r="H26" s="3">
         <v>208</v>
@@ -1873,30 +1933,30 @@
         <v>1</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>106</v>
+        <v>53</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="D27" s="2">
         <v>2152</v>
       </c>
-      <c r="E27" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>108</v>
+      <c r="E27" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="H27" s="3">
         <v>208</v>
@@ -1911,30 +1971,30 @@
         <v>1</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="D28" s="2">
         <v>2152</v>
       </c>
-      <c r="E28" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>112</v>
+      <c r="E28" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="H28" s="3">
         <v>208</v>
@@ -1949,30 +2009,30 @@
         <v>1</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>114</v>
+        <v>57</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>115</v>
+        <v>58</v>
       </c>
       <c r="D29" s="2">
         <v>2152</v>
       </c>
-      <c r="E29" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>116</v>
+      <c r="E29" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>138</v>
       </c>
       <c r="H29" s="3">
         <v>208</v>
@@ -1987,30 +2047,30 @@
         <v>1</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>118</v>
+        <v>59</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>119</v>
+        <v>60</v>
       </c>
       <c r="D30" s="2">
         <v>2152</v>
       </c>
-      <c r="E30" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>120</v>
+      <c r="E30" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="H30" s="3">
         <v>208</v>
@@ -2025,30 +2085,30 @@
         <v>1</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>121</v>
+        <v>61</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>122</v>
+        <v>62</v>
       </c>
       <c r="D31" s="2">
         <v>2152</v>
       </c>
-      <c r="E31" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>123</v>
+      <c r="E31" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="H31" s="3">
         <v>208</v>
@@ -2063,30 +2123,30 @@
         <v>1</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>125</v>
+        <v>64</v>
       </c>
       <c r="D32" s="2">
         <v>2152</v>
       </c>
-      <c r="E32" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>126</v>
+      <c r="E32" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="H32" s="3">
         <v>208</v>
@@ -2101,30 +2161,30 @@
         <v>1</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>127</v>
+        <v>65</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>128</v>
+        <v>66</v>
       </c>
       <c r="D33" s="2">
         <v>2152</v>
       </c>
-      <c r="E33" s="2">
-        <v>2152</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>129</v>
+      <c r="E33" s="4">
+        <v>2152</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>142</v>
       </c>
       <c r="H33" s="3">
         <v>208</v>
@@ -2139,11 +2199,12 @@
         <v>1</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>